<commit_message>
update regression and classification models
</commit_message>
<xml_diff>
--- a/machine_learning/data/template_raw.xlsx
+++ b/machine_learning/data/template_raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robinsse/Documents/github/gut_microbe_defluorination_paper/machine_learning/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336C822C-7E43-414A-A602-C65A53811BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2558D13-A4BC-244F-A730-893246893FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62640" yWindow="-9920" windowWidth="38160" windowHeight="17660" xr2:uid="{4C67F7C5-C32F-6B40-94D5-DA22915FCE92}"/>
+    <workbookView xWindow="67200" yWindow="-9920" windowWidth="33600" windowHeight="17660" xr2:uid="{4C67F7C5-C32F-6B40-94D5-DA22915FCE92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1161,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC1971C-B515-5A46-9FB2-DB5CAF6D50A8}">
   <dimension ref="A1:AL21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="143" workbookViewId="0">
+      <selection activeCell="AD6" sqref="AD6:AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>